<commit_message>
Ignorar pasta All_in e salvar alterações locais
</commit_message>
<xml_diff>
--- a/dados/silver/get_encerradas_info.xlsx
+++ b/dados/silver/get_encerradas_info.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1141" uniqueCount="691">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1141" uniqueCount="692">
   <si>
     <t>ID Campanha</t>
   </si>
@@ -1867,7 +1867,7 @@
     <t>44</t>
   </si>
   <si>
-    <t>3619</t>
+    <t>3620</t>
   </si>
   <si>
     <t>335</t>
@@ -1891,7 +1891,7 @@
     <t>13</t>
   </si>
   <si>
-    <t>3515</t>
+    <t>3518</t>
   </si>
   <si>
     <t>268</t>
@@ -1906,7 +1906,7 @@
     <t>24</t>
   </si>
   <si>
-    <t>3152</t>
+    <t>3155</t>
   </si>
   <si>
     <t>359</t>
@@ -1921,7 +1921,7 @@
     <t>127</t>
   </si>
   <si>
-    <t>3328</t>
+    <t>3330</t>
   </si>
   <si>
     <t>286</t>
@@ -1933,10 +1933,10 @@
     <t>352</t>
   </si>
   <si>
-    <t>3586</t>
-  </si>
-  <si>
-    <t>242</t>
+    <t>3587</t>
+  </si>
+  <si>
+    <t>243</t>
   </si>
   <si>
     <t>353</t>
@@ -1945,7 +1945,7 @@
     <t>84</t>
   </si>
   <si>
-    <t>2928</t>
+    <t>2934</t>
   </si>
   <si>
     <t>34</t>
@@ -1975,9 +1975,6 @@
     <t>289</t>
   </si>
   <si>
-    <t>365</t>
-  </si>
-  <si>
     <t>298</t>
   </si>
   <si>
@@ -1990,16 +1987,13 @@
     <t>318</t>
   </si>
   <si>
-    <t>3027</t>
-  </si>
-  <si>
-    <t>2153</t>
-  </si>
-  <si>
-    <t>358</t>
-  </si>
-  <si>
-    <t>89</t>
+    <t>3040</t>
+  </si>
+  <si>
+    <t>2159</t>
+  </si>
+  <si>
+    <t>91</t>
   </si>
   <si>
     <t>330</t>
@@ -2011,28 +2005,37 @@
     <t>332</t>
   </si>
   <si>
-    <t>2666</t>
+    <t>2697</t>
   </si>
   <si>
     <t>316</t>
   </si>
   <si>
-    <t>299</t>
-  </si>
-  <si>
-    <t>290</t>
-  </si>
-  <si>
-    <t>78</t>
-  </si>
-  <si>
-    <t>747</t>
-  </si>
-  <si>
-    <t>205</t>
-  </si>
-  <si>
-    <t>210</t>
+    <t>337</t>
+  </si>
+  <si>
+    <t>356</t>
+  </si>
+  <si>
+    <t>301</t>
+  </si>
+  <si>
+    <t>295</t>
+  </si>
+  <si>
+    <t>82</t>
+  </si>
+  <si>
+    <t>338</t>
+  </si>
+  <si>
+    <t>1894</t>
+  </si>
+  <si>
+    <t>285</t>
+  </si>
+  <si>
+    <t>276</t>
   </si>
   <si>
     <t>0</t>
@@ -2071,7 +2074,7 @@
     <t>113</t>
   </si>
   <si>
-    <t>410</t>
+    <t>411</t>
   </si>
   <si>
     <t>60</t>
@@ -2083,7 +2086,7 @@
     <t>401</t>
   </si>
   <si>
-    <t>271</t>
+    <t>279</t>
   </si>
   <si>
     <t>69</t>
@@ -2505,7 +2508,7 @@
         <v>532</v>
       </c>
       <c r="I2" t="s">
-        <v>673</v>
+        <v>674</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -2534,7 +2537,7 @@
         <v>601</v>
       </c>
       <c r="I3" t="s">
-        <v>674</v>
+        <v>675</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -2563,7 +2566,7 @@
         <v>499</v>
       </c>
       <c r="I4" t="s">
-        <v>673</v>
+        <v>674</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -2592,7 +2595,7 @@
         <v>530</v>
       </c>
       <c r="I5" t="s">
-        <v>673</v>
+        <v>674</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -2621,7 +2624,7 @@
         <v>539</v>
       </c>
       <c r="I6" t="s">
-        <v>673</v>
+        <v>674</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -2650,7 +2653,7 @@
         <v>602</v>
       </c>
       <c r="I7" t="s">
-        <v>673</v>
+        <v>674</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -2679,7 +2682,7 @@
         <v>603</v>
       </c>
       <c r="I8" t="s">
-        <v>673</v>
+        <v>674</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -2708,7 +2711,7 @@
         <v>604</v>
       </c>
       <c r="I9" t="s">
-        <v>673</v>
+        <v>674</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -2737,7 +2740,7 @@
         <v>533</v>
       </c>
       <c r="I10" t="s">
-        <v>673</v>
+        <v>674</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -2882,7 +2885,7 @@
         <v>542</v>
       </c>
       <c r="I15" t="s">
-        <v>673</v>
+        <v>674</v>
       </c>
     </row>
     <row r="16" spans="1:9">
@@ -3079,7 +3082,7 @@
         <v>606</v>
       </c>
       <c r="I22" t="s">
-        <v>675</v>
+        <v>676</v>
       </c>
     </row>
     <row r="23" spans="1:9">
@@ -3108,7 +3111,7 @@
         <v>607</v>
       </c>
       <c r="I23" t="s">
-        <v>673</v>
+        <v>674</v>
       </c>
     </row>
     <row r="24" spans="1:9">
@@ -3166,7 +3169,7 @@
         <v>609</v>
       </c>
       <c r="I25" t="s">
-        <v>673</v>
+        <v>674</v>
       </c>
     </row>
     <row r="26" spans="1:9">
@@ -3218,7 +3221,7 @@
         <v>530</v>
       </c>
       <c r="I27" t="s">
-        <v>673</v>
+        <v>674</v>
       </c>
     </row>
     <row r="28" spans="1:9">
@@ -3276,7 +3279,7 @@
         <v>519</v>
       </c>
       <c r="I29" t="s">
-        <v>673</v>
+        <v>674</v>
       </c>
     </row>
     <row r="30" spans="1:9">
@@ -3415,7 +3418,7 @@
         <v>612</v>
       </c>
       <c r="I34" t="s">
-        <v>673</v>
+        <v>674</v>
       </c>
     </row>
     <row r="35" spans="1:9">
@@ -3554,7 +3557,7 @@
         <v>604</v>
       </c>
       <c r="I39" t="s">
-        <v>673</v>
+        <v>674</v>
       </c>
     </row>
     <row r="40" spans="1:9">
@@ -3606,7 +3609,7 @@
         <v>613</v>
       </c>
       <c r="I41" t="s">
-        <v>673</v>
+        <v>674</v>
       </c>
     </row>
     <row r="42" spans="1:9">
@@ -3664,7 +3667,7 @@
         <v>542</v>
       </c>
       <c r="I43" t="s">
-        <v>673</v>
+        <v>674</v>
       </c>
     </row>
     <row r="44" spans="1:9">
@@ -3751,7 +3754,7 @@
         <v>604</v>
       </c>
       <c r="I46" t="s">
-        <v>673</v>
+        <v>674</v>
       </c>
     </row>
     <row r="47" spans="1:9">
@@ -3780,7 +3783,7 @@
         <v>542</v>
       </c>
       <c r="I47" t="s">
-        <v>673</v>
+        <v>674</v>
       </c>
     </row>
     <row r="48" spans="1:9">
@@ -3809,7 +3812,7 @@
         <v>542</v>
       </c>
       <c r="I48" t="s">
-        <v>673</v>
+        <v>674</v>
       </c>
     </row>
     <row r="49" spans="1:9">
@@ -3838,7 +3841,7 @@
         <v>613</v>
       </c>
       <c r="I49" t="s">
-        <v>676</v>
+        <v>677</v>
       </c>
     </row>
     <row r="50" spans="1:9">
@@ -3867,7 +3870,7 @@
         <v>542</v>
       </c>
       <c r="I50" t="s">
-        <v>673</v>
+        <v>674</v>
       </c>
     </row>
     <row r="51" spans="1:9">
@@ -3983,7 +3986,7 @@
         <v>617</v>
       </c>
       <c r="I54" t="s">
-        <v>677</v>
+        <v>678</v>
       </c>
     </row>
     <row r="55" spans="1:9">
@@ -4070,7 +4073,7 @@
         <v>530</v>
       </c>
       <c r="I57" t="s">
-        <v>673</v>
+        <v>674</v>
       </c>
     </row>
     <row r="58" spans="1:9">
@@ -4296,7 +4299,7 @@
         <v>621</v>
       </c>
       <c r="I65" t="s">
-        <v>673</v>
+        <v>674</v>
       </c>
     </row>
     <row r="66" spans="1:9">
@@ -4325,7 +4328,7 @@
         <v>622</v>
       </c>
       <c r="I66" t="s">
-        <v>673</v>
+        <v>674</v>
       </c>
     </row>
     <row r="67" spans="1:9">
@@ -4441,7 +4444,7 @@
         <v>542</v>
       </c>
       <c r="I70" t="s">
-        <v>673</v>
+        <v>674</v>
       </c>
     </row>
     <row r="71" spans="1:9">
@@ -4470,7 +4473,7 @@
         <v>603</v>
       </c>
       <c r="I71" t="s">
-        <v>673</v>
+        <v>674</v>
       </c>
     </row>
     <row r="72" spans="1:9">
@@ -4499,7 +4502,7 @@
         <v>604</v>
       </c>
       <c r="I72" t="s">
-        <v>673</v>
+        <v>674</v>
       </c>
     </row>
     <row r="73" spans="1:9">
@@ -4528,7 +4531,7 @@
         <v>603</v>
       </c>
       <c r="I73" t="s">
-        <v>673</v>
+        <v>674</v>
       </c>
     </row>
     <row r="74" spans="1:9">
@@ -4557,7 +4560,7 @@
         <v>625</v>
       </c>
       <c r="I74" t="s">
-        <v>673</v>
+        <v>674</v>
       </c>
     </row>
     <row r="75" spans="1:9">
@@ -4586,7 +4589,7 @@
         <v>626</v>
       </c>
       <c r="I75" t="s">
-        <v>678</v>
+        <v>679</v>
       </c>
     </row>
     <row r="76" spans="1:9">
@@ -4615,7 +4618,7 @@
         <v>533</v>
       </c>
       <c r="I76" t="s">
-        <v>673</v>
+        <v>674</v>
       </c>
     </row>
     <row r="77" spans="1:9">
@@ -4644,7 +4647,7 @@
         <v>513</v>
       </c>
       <c r="I77" t="s">
-        <v>673</v>
+        <v>674</v>
       </c>
     </row>
     <row r="78" spans="1:9">
@@ -4673,7 +4676,7 @@
         <v>627</v>
       </c>
       <c r="I78" t="s">
-        <v>679</v>
+        <v>680</v>
       </c>
     </row>
     <row r="79" spans="1:9">
@@ -4702,7 +4705,7 @@
         <v>628</v>
       </c>
       <c r="I79" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
     </row>
     <row r="80" spans="1:9">
@@ -4760,7 +4763,7 @@
         <v>630</v>
       </c>
       <c r="I81" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
     </row>
     <row r="82" spans="1:9">
@@ -4876,7 +4879,7 @@
         <v>603</v>
       </c>
       <c r="I85" t="s">
-        <v>673</v>
+        <v>674</v>
       </c>
     </row>
     <row r="86" spans="1:9">
@@ -4934,7 +4937,7 @@
         <v>635</v>
       </c>
       <c r="I87" t="s">
-        <v>673</v>
+        <v>674</v>
       </c>
     </row>
     <row r="88" spans="1:9">
@@ -4963,7 +4966,7 @@
         <v>636</v>
       </c>
       <c r="I88" t="s">
-        <v>673</v>
+        <v>674</v>
       </c>
     </row>
     <row r="89" spans="1:9">
@@ -4992,7 +4995,7 @@
         <v>496</v>
       </c>
       <c r="I89" t="s">
-        <v>673</v>
+        <v>674</v>
       </c>
     </row>
     <row r="90" spans="1:9">
@@ -5021,7 +5024,7 @@
         <v>584</v>
       </c>
       <c r="I90" t="s">
-        <v>673</v>
+        <v>674</v>
       </c>
     </row>
     <row r="91" spans="1:9">
@@ -5050,7 +5053,7 @@
         <v>637</v>
       </c>
       <c r="I91" t="s">
-        <v>682</v>
+        <v>683</v>
       </c>
     </row>
     <row r="92" spans="1:9">
@@ -5108,7 +5111,7 @@
         <v>524</v>
       </c>
       <c r="I93" t="s">
-        <v>683</v>
+        <v>684</v>
       </c>
     </row>
     <row r="94" spans="1:9">
@@ -5137,7 +5140,7 @@
         <v>629</v>
       </c>
       <c r="I94" t="s">
-        <v>676</v>
+        <v>677</v>
       </c>
     </row>
     <row r="95" spans="1:9">
@@ -5166,7 +5169,7 @@
         <v>610</v>
       </c>
       <c r="I95" t="s">
-        <v>676</v>
+        <v>677</v>
       </c>
     </row>
     <row r="96" spans="1:9">
@@ -5224,7 +5227,7 @@
         <v>639</v>
       </c>
       <c r="I97" t="s">
-        <v>673</v>
+        <v>674</v>
       </c>
     </row>
     <row r="98" spans="1:9">
@@ -5369,7 +5372,7 @@
         <v>641</v>
       </c>
       <c r="I102" t="s">
-        <v>684</v>
+        <v>685</v>
       </c>
     </row>
     <row r="103" spans="1:9">
@@ -5427,7 +5430,7 @@
         <v>643</v>
       </c>
       <c r="I104" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
     </row>
     <row r="105" spans="1:9">
@@ -5456,7 +5459,7 @@
         <v>644</v>
       </c>
       <c r="I105" t="s">
-        <v>683</v>
+        <v>684</v>
       </c>
     </row>
     <row r="106" spans="1:9">
@@ -5572,7 +5575,7 @@
         <v>506</v>
       </c>
       <c r="I109" t="s">
-        <v>673</v>
+        <v>674</v>
       </c>
     </row>
     <row r="110" spans="1:9">
@@ -5630,7 +5633,7 @@
         <v>647</v>
       </c>
       <c r="I111" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
     </row>
     <row r="112" spans="1:9">
@@ -5659,7 +5662,7 @@
         <v>648</v>
       </c>
       <c r="I112" t="s">
-        <v>683</v>
+        <v>684</v>
       </c>
     </row>
     <row r="113" spans="1:9">
@@ -5688,7 +5691,7 @@
         <v>649</v>
       </c>
       <c r="I113" t="s">
-        <v>683</v>
+        <v>684</v>
       </c>
     </row>
     <row r="114" spans="1:9">
@@ -5717,7 +5720,7 @@
         <v>499</v>
       </c>
       <c r="I114" t="s">
-        <v>673</v>
+        <v>674</v>
       </c>
     </row>
     <row r="115" spans="1:9">
@@ -5775,7 +5778,7 @@
         <v>651</v>
       </c>
       <c r="I116" t="s">
-        <v>678</v>
+        <v>679</v>
       </c>
     </row>
     <row r="117" spans="1:9">
@@ -5830,7 +5833,7 @@
         <v>928</v>
       </c>
       <c r="H118" t="s">
-        <v>653</v>
+        <v>645</v>
       </c>
       <c r="I118" t="s">
         <v>510</v>
@@ -5888,7 +5891,7 @@
         <v>1966</v>
       </c>
       <c r="H120" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="I120" t="s">
         <v>604</v>
@@ -5917,7 +5920,7 @@
         <v>934</v>
       </c>
       <c r="H121" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="I121" t="s">
         <v>520</v>
@@ -5949,7 +5952,7 @@
         <v>533</v>
       </c>
       <c r="I122" t="s">
-        <v>673</v>
+        <v>674</v>
       </c>
     </row>
     <row r="123" spans="1:9">
@@ -5975,10 +5978,10 @@
         <v>934</v>
       </c>
       <c r="H123" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="I123" t="s">
-        <v>687</v>
+        <v>688</v>
       </c>
     </row>
     <row r="124" spans="1:9">
@@ -6004,7 +6007,7 @@
         <v>1357</v>
       </c>
       <c r="H124" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="I124" t="s">
         <v>530</v>
@@ -6033,10 +6036,10 @@
         <v>50275</v>
       </c>
       <c r="H125" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="I125" t="s">
-        <v>688</v>
+        <v>689</v>
       </c>
     </row>
     <row r="126" spans="1:9">
@@ -6062,7 +6065,7 @@
         <v>43125</v>
       </c>
       <c r="H126" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="I126" t="s">
         <v>551</v>
@@ -6091,7 +6094,7 @@
         <v>935</v>
       </c>
       <c r="H127" t="s">
-        <v>660</v>
+        <v>631</v>
       </c>
       <c r="I127" t="s">
         <v>520</v>
@@ -6120,10 +6123,10 @@
         <v>375</v>
       </c>
       <c r="H128" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
       <c r="I128" t="s">
-        <v>673</v>
+        <v>674</v>
       </c>
     </row>
     <row r="129" spans="1:9">
@@ -6149,10 +6152,10 @@
         <v>934</v>
       </c>
       <c r="H129" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
       <c r="I129" t="s">
-        <v>683</v>
+        <v>684</v>
       </c>
     </row>
     <row r="130" spans="1:9">
@@ -6178,7 +6181,7 @@
         <v>934</v>
       </c>
       <c r="H130" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="I130" t="s">
         <v>498</v>
@@ -6207,7 +6210,7 @@
         <v>1356</v>
       </c>
       <c r="H131" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
       <c r="I131" t="s">
         <v>612</v>
@@ -6239,7 +6242,7 @@
         <v>513</v>
       </c>
       <c r="I132" t="s">
-        <v>673</v>
+        <v>674</v>
       </c>
     </row>
     <row r="133" spans="1:9">
@@ -6265,10 +6268,10 @@
         <v>50655</v>
       </c>
       <c r="H133" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="I133" t="s">
-        <v>689</v>
+        <v>690</v>
       </c>
     </row>
     <row r="134" spans="1:9">
@@ -6323,10 +6326,10 @@
         <v>1354</v>
       </c>
       <c r="H135" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="I135" t="s">
-        <v>683</v>
+        <v>684</v>
       </c>
     </row>
     <row r="136" spans="1:9">
@@ -6352,7 +6355,7 @@
         <v>1352</v>
       </c>
       <c r="H136" t="s">
-        <v>646</v>
+        <v>665</v>
       </c>
       <c r="I136" t="s">
         <v>513</v>
@@ -6381,7 +6384,7 @@
         <v>934</v>
       </c>
       <c r="H137" t="s">
-        <v>641</v>
+        <v>666</v>
       </c>
       <c r="I137" t="s">
         <v>511</v>
@@ -6413,7 +6416,7 @@
         <v>667</v>
       </c>
       <c r="I138" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
     </row>
     <row r="139" spans="1:9">
@@ -6436,7 +6439,7 @@
         <v>597</v>
       </c>
       <c r="G139">
-        <v>932</v>
+        <v>901</v>
       </c>
       <c r="H139" t="s">
         <v>668</v>
@@ -6497,7 +6500,7 @@
         <v>898</v>
       </c>
       <c r="H141" t="s">
-        <v>646</v>
+        <v>670</v>
       </c>
       <c r="I141" t="s">
         <v>520</v>
@@ -6523,13 +6526,13 @@
         <v>598</v>
       </c>
       <c r="G142">
-        <v>51902</v>
+        <v>50641</v>
       </c>
       <c r="H142" t="s">
-        <v>670</v>
+        <v>671</v>
       </c>
       <c r="I142" t="s">
-        <v>624</v>
+        <v>629</v>
       </c>
     </row>
     <row r="143" spans="1:9">
@@ -6555,10 +6558,10 @@
         <v>1362</v>
       </c>
       <c r="H143" t="s">
-        <v>671</v>
+        <v>672</v>
       </c>
       <c r="I143" t="s">
-        <v>673</v>
+        <v>604</v>
       </c>
     </row>
     <row r="144" spans="1:9">
@@ -6584,7 +6587,7 @@
         <v>1352</v>
       </c>
       <c r="H144" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="I144" t="s">
         <v>530</v>

</xml_diff>